<commit_message>
Got openpyslx to read rows starting at sample info and append to empty list a dict of sample if that be used to generate whole statement block
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -28,15 +28,36 @@
     <t xml:space="preserve">betzjwx_ELN_AttemptID</t>
   </si>
   <si>
+    <t xml:space="preserve">Sample Set ID: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example ID XXXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result Set ID:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARD/NCE_2024/Rest/Of/Path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target-Analyte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-1968666.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APQL:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample #:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample Set data</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample Set ID: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Example ID XXXXXX</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
   <si>
@@ -55,9 +76,6 @@
     <t xml:space="preserve">Other peak(s) Give as comma sperated values of conc</t>
   </si>
   <si>
-    <t xml:space="preserve">Result Set ID:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blank</t>
   </si>
   <si>
@@ -70,12 +88,6 @@
     <t xml:space="preserve">6.23, 2.15, 0.015, 8.23</t>
   </si>
   <si>
-    <t xml:space="preserve">Path: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARD/NCE_2024/Rest/Of/Path</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sample  </t>
   </si>
   <si>
@@ -85,12 +97,6 @@
     <t xml:space="preserve">Fail</t>
   </si>
   <si>
-    <t xml:space="preserve">Target-Analyte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A-1968666.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Delrin</t>
   </si>
   <si>
@@ -98,12 +104,6 @@
   </si>
   <si>
     <t xml:space="preserve">etc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APQL:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sample #:</t>
   </si>
 </sst>
 </file>
@@ -198,16 +198,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -399,191 +399,240 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="52.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="63.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="63.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E4" s="0"/>
+      <c r="F4" s="0"/>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+      <c r="I4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+      <c r="I5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="B6" s="2" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="B7" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F12" s="2" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="n">
+      <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Reworked funcs of practice, will rename as final project. Added dedicated function that gathers sample data and arranges into a list of dicts
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t xml:space="preserve">Sample Set:</t>
   </si>
@@ -28,33 +28,54 @@
     <t xml:space="preserve">betzjwx_ELN_AttemptID</t>
   </si>
   <si>
+    <t xml:space="preserve">Swab Material APQLs (ug/100cm2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample Set ID: </t>
   </si>
   <si>
     <t xml:space="preserve">Example ID XXXXXX</t>
   </si>
   <si>
+    <t xml:space="preserve">Stainless Steel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Result Set ID:</t>
   </si>
   <si>
+    <t xml:space="preserve">Delrin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Path: </t>
   </si>
   <si>
     <t xml:space="preserve">ARD/NCE_2024/Rest/Of/Path</t>
   </si>
   <si>
+    <t xml:space="preserve">Nickel</t>
+  </si>
+  <si>
     <t xml:space="preserve">Target-Analyte</t>
   </si>
   <si>
     <t xml:space="preserve">A-1968666.0</t>
   </si>
   <si>
-    <t xml:space="preserve">APQL:</t>
+    <t xml:space="preserve">Chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APQL (For Rinse Only, if swabs are marked yes this box will be ignored:</t>
   </si>
   <si>
     <t xml:space="preserve">Sample #:</t>
   </si>
   <si>
+    <t xml:space="preserve">Swabs? Leave yes or no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample Set data</t>
   </si>
   <si>
@@ -91,13 +112,7 @@
     <t xml:space="preserve">Sample  </t>
   </si>
   <si>
-    <t xml:space="preserve">Stainless Steel</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delrin</t>
   </si>
   <si>
     <t xml:space="preserve">et</t>
@@ -193,7 +208,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -207,6 +222,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,10 +426,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -422,217 +449,229 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>1.25</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>1.11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="0"/>
-      <c r="F4" s="0"/>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
+        <v>9</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>1.16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.016</v>
       </c>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>15</v>
-      </c>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
+        <v>20</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="2" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A9:F9"/>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="A12:F12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Working on statment generator
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -479,7 +479,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>1.11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Further progress with building statment generator
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -429,7 +429,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,7 +515,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.016</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>

</xml_diff>

<commit_message>
Finished blank rinse samples
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413234C9-DFD8-416F-9F16-A0D868689614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A752C8B-37FA-4639-B24F-BA9D07873975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24420" yWindow="795" windowWidth="18900" windowHeight="10965" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Sample Set:</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>6.23, 2.15, 0.015, 8.23</t>
@@ -183,14 +180,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,8 +383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -401,230 +398,235 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>1.25</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="1">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="1">
+        <v>25</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="3">
+    </row>
+    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1">
         <v>0.16</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F15" s="1">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
-        <v>2</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="C16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.16</v>
-      </c>
-      <c r="F15" s="3">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
-        <v>3</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
-        <v>4</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
-        <v>5</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="3"/>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Made statement generators their own module and just import the funcitons as needed
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A752C8B-37FA-4639-B24F-BA9D07873975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BAD518-37E3-4ACD-9E93-E287ABE387BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24420" yWindow="795" windowWidth="18900" windowHeight="10965" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="18900" windowHeight="10965" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Sample Set:</t>
   </si>
@@ -111,16 +111,22 @@
     <t xml:space="preserve">Sample  </t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>et</t>
-  </si>
-  <si>
     <t>etc</t>
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample </t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>fail</t>
   </si>
 </sst>
 </file>
@@ -176,18 +182,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,18 +390,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" customWidth="1"/>
-    <col min="6" max="6" width="63.28515625" customWidth="1"/>
-    <col min="7" max="7" width="52.42578125" customWidth="1"/>
-    <col min="8" max="9" width="63.5703125" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="2"/>
+    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="63.5703125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="12.5703125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
@@ -404,10 +413,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -416,10 +425,10 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="4">
         <v>1.25</v>
       </c>
     </row>
@@ -430,10 +439,10 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="4">
         <v>20</v>
       </c>
     </row>
@@ -444,10 +453,10 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="4">
         <v>1.1599999999999999</v>
       </c>
     </row>
@@ -455,25 +464,25 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="4">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -482,22 +491,22 @@
       <c r="B7" s="1">
         <v>20</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F10" s="1" t="s">
@@ -505,14 +514,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -545,10 +554,10 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>26</v>
@@ -559,36 +568,34 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E15" s="1">
-        <v>0.16</v>
-      </c>
-      <c r="F15" s="1">
-        <v>2.1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -600,13 +607,13 @@
         <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -618,13 +625,13 @@
         <v>27</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F18" s="1"/>
     </row>

</xml_diff>

<commit_message>
Finalized statement genorator for rinse samples, also altered how sample list is generated that way empty cells in sample ID and type are not appended to the sample list
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETZJWX\Documents\CS50P-Work-Folder-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BAD518-37E3-4ACD-9E93-E287ABE387BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3BF12A-7C57-4A9B-B431-A05BA112EE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="18900" windowHeight="10965" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>Sample Set:</t>
   </si>
@@ -108,25 +108,19 @@
     <t>6.23, 2.15, 0.015, 8.23</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample  </t>
-  </si>
-  <si>
-    <t>etc</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>Pass</t>
   </si>
   <si>
-    <t xml:space="preserve">Sample </t>
-  </si>
-  <si>
     <t>sample</t>
   </si>
   <si>
-    <t>fail</t>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>100041567 LC80277</t>
   </si>
 </sst>
 </file>
@@ -182,19 +176,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,22 +381,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" style="2"/>
-    <col min="5" max="5" width="21.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="63.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="52.42578125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="63.5703125" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="12.5703125" style="2"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="63.28515625" customWidth="1"/>
+    <col min="7" max="7" width="52.42578125" customWidth="1"/>
+    <col min="8" max="9" width="63.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
@@ -413,10 +404,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -425,10 +416,10 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2">
         <v>1.25</v>
       </c>
     </row>
@@ -439,10 +430,10 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <v>20</v>
       </c>
     </row>
@@ -453,10 +444,10 @@
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <v>1.1599999999999999</v>
       </c>
     </row>
@@ -464,25 +455,25 @@
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>20</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -491,22 +482,22 @@
       <c r="B7" s="1">
         <v>20</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="F10" s="1" t="s">
@@ -514,14 +505,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -544,8 +535,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1</v>
+      <c r="A14" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
@@ -554,7 +545,7 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -568,72 +559,84 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>3</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
       <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Updated swab generation to handle none values for A result for blank swabs
</commit_message>
<xml_diff>
--- a/Cleaning Samples Template.xlsx
+++ b/Cleaning Samples Template.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t xml:space="preserve">Sample Set:</t>
   </si>
@@ -112,10 +112,25 @@
     <t xml:space="preserve">Pass</t>
   </si>
   <si>
-    <t xml:space="preserve">sample</t>
+    <t xml:space="preserve">blank</t>
   </si>
   <si>
     <t xml:space="preserve">pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delrin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nickel</t>
   </si>
 </sst>
 </file>
@@ -205,24 +220,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -418,262 +437,304 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="63.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="52.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="63.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="63.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="52.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="63.57"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="3" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="3" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="3" t="n">
         <v>1.16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="3" t="n">
         <v>1.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>7.18</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E18" s="2" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>